<commit_message>
fixed issues with error handling
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\BCIT Work Synced Folder\My Courses\COMP3522 OOP 2\Winter 2020\Assignments\Assignment 2 Supply Chain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonl\ShareFile\Personal Folders\Term_3\COMP_3522\3522_A01062166\Assignments\Assignment_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F959E200-ABA9-4C24-84DC-7F0EB85250A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FD7AFC-5F9F-46C2-96E2-B8AB0DB88417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="19170" windowHeight="10770" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,9 +186,6 @@
     <t>E9451C</t>
   </si>
   <si>
-    <t>H4443S</t>
-  </si>
-  <si>
     <t>C8311S</t>
   </si>
   <si>
@@ -307,6 +304,9 @@
   </si>
   <si>
     <t>Sea Salt</t>
+  </si>
+  <si>
+    <t>14443S</t>
   </si>
 </sst>
 </file>
@@ -663,9 +663,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC969572-FB28-418E-B89D-F0DD002AE5AA}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T14" sqref="T14"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,28 +810,28 @@
         <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V3" t="s">
+        <v>78</v>
+      </c>
+      <c r="W3" t="s">
         <v>79</v>
       </c>
-      <c r="W3" t="s">
-        <v>80</v>
-      </c>
       <c r="X3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -889,7 +889,7 @@
         <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -901,7 +901,7 @@
         <v>30</v>
       </c>
       <c r="Q5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -924,7 +924,7 @@
         <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H6" t="s">
         <v>34</v>
@@ -956,7 +956,7 @@
         <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -965,7 +965,7 @@
         <v>50</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R7" t="s">
         <v>34</v>
@@ -988,28 +988,28 @@
         <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N8" t="s">
         <v>34</v>
       </c>
       <c r="V8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -1023,28 +1023,28 @@
         <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N9" t="s">
         <v>34</v>
       </c>
       <c r="V9" t="s">
+        <v>86</v>
+      </c>
+      <c r="W9" t="s">
+        <v>80</v>
+      </c>
+      <c r="X9" t="s">
         <v>87</v>
-      </c>
-      <c r="W9" t="s">
-        <v>81</v>
-      </c>
-      <c r="X9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -1058,19 +1058,19 @@
         <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10">
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R10" t="s">
         <v>33</v>
@@ -1090,28 +1090,28 @@
         <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11">
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -1134,7 +1134,7 @@
         <v>31</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H12" t="s">
         <v>34</v>
@@ -1175,7 +1175,7 @@
         <v>32</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H13" t="s">
         <v>34</v>
@@ -1207,19 +1207,19 @@
         <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14">
         <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R14" t="s">
         <v>33</v>
@@ -1239,16 +1239,16 @@
         <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15">
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R15" t="s">
         <v>34</v>
@@ -1257,7 +1257,7 @@
         <v>34</v>
       </c>
       <c r="T15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>